<commit_message>
Added: 1) Navigation from MyProfileView to ChangePasswordForm
</commit_message>
<xml_diff>
--- a/data/user/UserLogin.xlsx
+++ b/data/user/UserLogin.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grey Bunny\Desktop\FCS5-Grp5\data\user\"/>
     </mc:Choice>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t>uid</t>
   </si>
@@ -64,12 +64,16 @@
   </si>
   <si>
     <t>S3456789E</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -234,129 +238,129 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="4.0"/>
+    <col min="2" max="2" customWidth="true" width="10.5703125"/>
+    <col min="3" max="3" customWidth="true" width="9.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="0">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" s="0">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="A7" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="B7" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
-        <v>2</v>
+      <c r="C7" t="s" s="0">
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="0">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="A11" s="0">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>2</v>
       </c>
     </row>

</xml_diff>